<commit_message>
updating bug in correction rules
</commit_message>
<xml_diff>
--- a/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Core QC Rules/BCRPP Correction Rules.xlsx
+++ b/BCRPP_QC_R_Excel_Program/BCRPP_QC_Version_1/Core QC Rules/BCRPP Correction Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955584E1-DACF-F749-8939-EF40AC879E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E80CBE5-2DA2-B64C-BD88-26667C68139B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40960" yWindow="800" windowWidth="40960" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="139">
   <si>
     <t>variable</t>
   </si>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView tabSelected="1" topLeftCell="K33" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2091,6 +2091,9 @@
       <c r="B47" s="1">
         <v>777</v>
       </c>
+      <c r="C47" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L47" s="1">
         <v>7777</v>
       </c>
@@ -2104,6 +2107,9 @@
       </c>
       <c r="B48" s="1">
         <v>888</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="L48" s="1">
         <v>8888</v>

</xml_diff>